<commit_message>
Added RST+TX+RX to Expansion Header
Added RST, and Serial TXD/RXD to the Expansion header. To allow TXD/RXD from the FT232RL to be safely 'overriden' by an expansion device, two additional 1K resistors have been fitted as well.
</commit_message>
<xml_diff>
--- a/hardware/Parts List.xlsx
+++ b/hardware/Parts List.xlsx
@@ -217,9 +217,6 @@
     <t>R16</t>
   </si>
   <si>
-    <t>R18, R25-R26</t>
-  </si>
-  <si>
     <t>R19</t>
   </si>
   <si>
@@ -397,18 +394,6 @@
     <t>Samtec</t>
   </si>
   <si>
-    <t>SSW-104-01-T-S</t>
-  </si>
-  <si>
-    <t>200-SSW10401TS</t>
-  </si>
-  <si>
-    <t>1803393</t>
-  </si>
-  <si>
-    <t>1x04 2.54mm Square Header Recepticle, Vertical, THT</t>
-  </si>
-  <si>
     <t>DS1a</t>
   </si>
   <si>
@@ -928,9 +913,6 @@
     <t>Connector_IDC:IDC-Header_2x03_P2.54mm_Vertical</t>
   </si>
   <si>
-    <t>Connector_PinSocket_2.54mm:PinSocket_1x04_P2.54mm_Vertical</t>
-  </si>
-  <si>
     <t>Buzzer_Beeper:Buzzer_15x7.5RM7.6</t>
   </si>
   <si>
@@ -959,6 +941,24 @@
   </si>
   <si>
     <t>C1, C7-C15</t>
+  </si>
+  <si>
+    <t>SSW-107-01-T-S</t>
+  </si>
+  <si>
+    <t>200-SSW10701TS</t>
+  </si>
+  <si>
+    <t>2667434</t>
+  </si>
+  <si>
+    <t>1x07 2.54mm Square Header Recepticle, Vertical, THT</t>
+  </si>
+  <si>
+    <t>Connector_PinSocket_2.54mm:PinSocket_1x07_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>R18, R25-R26, R31-R32</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +1378,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,13 +1408,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>43</v>
@@ -1463,14 +1463,14 @@
         <v>44</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1505,10 +1505,10 @@
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1519,7 +1519,7 @@
         <v>46</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -1536,28 +1536,28 @@
         <v>0.32099999999999995</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="3">
         <v>44</v>
@@ -1574,28 +1574,28 @@
         <v>3.9820000000000002</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D6" s="3">
         <v>10</v>
@@ -1612,17 +1612,17 @@
         <v>1.4000000000000001</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1630,10 +1630,10 @@
         <v>57</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -1650,15 +1650,15 @@
         <v>1.3900000000000001</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="8" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1666,10 +1666,10 @@
         <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D8" s="3">
         <v>2</v>
@@ -1686,17 +1686,17 @@
         <v>0.66</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="8" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1704,10 +1704,10 @@
         <v>56</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
@@ -1724,15 +1724,15 @@
         <v>1.2</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="8" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1767,21 +1767,21 @@
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
@@ -1798,28 +1798,28 @@
         <v>0.38500000000000001</v>
       </c>
       <c r="H11" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>90</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
@@ -1836,26 +1836,26 @@
         <v>1.085</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
@@ -1872,26 +1872,26 @@
         <v>1.085</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D14" s="3">
         <v>1</v>
@@ -1908,7 +1908,7 @@
         <v>52.75</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -1916,18 +1916,18 @@
         <v>50</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
@@ -1945,25 +1945,25 @@
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="11" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="D16" s="3">
         <v>1</v>
@@ -1981,25 +1981,25 @@
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D17" s="3">
         <v>2</v>
@@ -2016,28 +2016,28 @@
         <v>3.37</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D18" s="3">
         <v>2</v>
@@ -2054,28 +2054,28 @@
         <v>2.06</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J18" s="7"/>
       <c r="K18" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
@@ -2092,28 +2092,28 @@
         <v>1.6500000000000001</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
@@ -2130,28 +2130,28 @@
         <v>0.96</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J20" s="7"/>
       <c r="K20" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
@@ -2168,28 +2168,28 @@
         <v>0.42500000000000004</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="7" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
@@ -2206,28 +2206,28 @@
         <v>3.5049999999999999</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="7" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
@@ -2244,26 +2244,26 @@
         <v>2.09</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
@@ -2281,25 +2281,25 @@
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="11" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="7" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>126</v>
+        <v>308</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
@@ -2309,24 +2309,24 @@
         <v>5</v>
       </c>
       <c r="F25" s="1">
-        <v>0.58799999999999997</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="1"/>
-        <v>2.94</v>
+        <v>3.6749999999999998</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>127</v>
+        <v>309</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>128</v>
+        <v>310</v>
       </c>
       <c r="J25" s="7"/>
       <c r="K25" s="7" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>129</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2359,21 +2359,21 @@
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
@@ -2390,15 +2390,15 @@
         <v>11.45</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2433,10 +2433,10 @@
       </c>
       <c r="J28" s="7"/>
       <c r="K28" s="7" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2471,10 +2471,10 @@
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="8" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2482,10 +2482,10 @@
         <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -2502,17 +2502,17 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J30" s="7"/>
       <c r="K30" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2520,10 +2520,10 @@
         <v>63</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D31" s="3">
         <v>6</v>
@@ -2540,17 +2540,17 @@
         <v>0.42</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="J31" s="7"/>
       <c r="K31" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2558,10 +2558,10 @@
         <v>64</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
@@ -2578,17 +2578,17 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="J32" s="7"/>
       <c r="K32" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2596,10 +2596,10 @@
         <v>65</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D33" s="3">
         <v>1</v>
@@ -2616,66 +2616,66 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J33" s="7"/>
       <c r="K33" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>66</v>
+        <v>313</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D34" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E34" s="3">
         <f t="shared" ref="E34:E54" si="2">D34*$G$56</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F34" s="1">
         <v>1.4E-2</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" si="1"/>
-        <v>0.21</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="J34" s="7"/>
       <c r="K34" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D35" s="3">
         <v>1</v>
@@ -2692,17 +2692,17 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="J35" s="7"/>
       <c r="K35" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2710,10 +2710,10 @@
         <v>59</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D36" s="3">
         <v>1</v>
@@ -2730,28 +2730,28 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="J36" s="7"/>
       <c r="K36" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D37" s="3">
         <v>2</v>
@@ -2768,28 +2768,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="J37" s="7"/>
       <c r="K37" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D38" s="3">
         <v>1</v>
@@ -2806,17 +2806,17 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H38" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="I38" s="7" t="s">
         <v>227</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>232</v>
       </c>
       <c r="J38" s="7"/>
       <c r="K38" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2824,10 +2824,10 @@
         <v>60</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D39" s="3">
         <v>3</v>
@@ -2844,17 +2844,17 @@
         <v>0.21</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J39" s="7"/>
       <c r="K39" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2862,10 +2862,10 @@
         <v>61</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D40" s="3">
         <v>7</v>
@@ -2882,17 +2882,17 @@
         <v>0.49</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="J40" s="7"/>
       <c r="K40" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2900,10 +2900,10 @@
         <v>62</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D41" s="3">
         <v>3</v>
@@ -2920,28 +2920,28 @@
         <v>0.18</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="J41" s="7"/>
       <c r="K41" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D42" s="3">
         <v>2</v>
@@ -2958,28 +2958,28 @@
         <v>2.79</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="J42" s="7"/>
       <c r="K42" s="7" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="D43" s="3">
         <v>1</v>
@@ -2996,17 +2996,17 @@
         <v>1.9</v>
       </c>
       <c r="H43" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I43" s="11" t="s">
         <v>98</v>
-      </c>
-      <c r="I43" s="11" t="s">
-        <v>99</v>
       </c>
       <c r="J43" s="7"/>
       <c r="K43" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -3042,18 +3042,18 @@
         <v>50</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="C45" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D45" s="3">
         <v>5</v>
@@ -3073,24 +3073,24 @@
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
       <c r="J45" s="14" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="K45" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D46" s="3">
         <v>5</v>
@@ -3107,28 +3107,28 @@
         <v>5.9249999999999998</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J46" s="7"/>
       <c r="K46" s="7" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D47" s="3">
         <v>5</v>
@@ -3145,28 +3145,28 @@
         <v>2.65</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="J47" s="7"/>
       <c r="K47" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D48" s="3">
         <v>1</v>
@@ -3183,26 +3183,26 @@
         <v>6.5</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
       <c r="K48" s="7" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D49" s="3">
         <v>1</v>
@@ -3219,17 +3219,17 @@
         <v>7.5</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="J49" s="7"/>
       <c r="K49" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3264,10 +3264,10 @@
       </c>
       <c r="J50" s="10"/>
       <c r="K50" s="17" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -3302,21 +3302,21 @@
       </c>
       <c r="J51" s="7"/>
       <c r="K51" s="7" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D52" s="3">
         <v>1</v>
@@ -3333,16 +3333,16 @@
         <v>17.399999999999999</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -3377,21 +3377,21 @@
       </c>
       <c r="J53" s="7"/>
       <c r="K53" s="17" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D54" s="3">
         <v>1</v>
@@ -3408,18 +3408,18 @@
         <v>1.7799999999999998</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F56" s="4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="G56" s="16">
         <v>5</v>
@@ -3431,16 +3431,16 @@
       </c>
       <c r="G57" s="5">
         <f>SUM(G2:G55)</f>
-        <v>290.70799999999997</v>
+        <v>291.58299999999991</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F58" s="4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="G58" s="5">
         <f>G57/G56</f>
-        <v>58.141599999999997</v>
+        <v>58.31659999999998</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Correction to Parts List, Starting on Interface Program
Interface Program now has ability to detect the addition and removal of individual USB Serial devices, and detect  their COM Port number and Serial Numbers
</commit_message>
<xml_diff>
--- a/hardware/Parts List.xlsx
+++ b/hardware/Parts List.xlsx
@@ -61,9 +61,6 @@
     <t>FM24C16B-G</t>
   </si>
   <si>
-    <t>877-FM24CL16B-G</t>
-  </si>
-  <si>
     <t>Footprint</t>
   </si>
   <si>
@@ -538,12 +535,6 @@
     <t>IQD</t>
   </si>
   <si>
-    <t>LFXTAL027945Bulk</t>
-  </si>
-  <si>
-    <t>449-LFXTAL027945BULK</t>
-  </si>
-  <si>
     <t>Parallel Crystal, 16MHz, 22pF, THT</t>
   </si>
   <si>
@@ -959,6 +950,15 @@
   </si>
   <si>
     <t>R18, R25-R26, R31-R32</t>
+  </si>
+  <si>
+    <t>877-FM24C16B-G</t>
+  </si>
+  <si>
+    <t>LFXTAL027945Reel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">449-LFXTAL027945REEL </t>
   </si>
 </sst>
 </file>
@@ -1047,9 +1047,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
@@ -1065,6 +1062,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1376,9 +1374,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,13 +1406,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -1429,7 +1427,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>2</v>
@@ -1437,13 +1435,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>42</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -1459,29 +1457,29 @@
         <f>E2*F2</f>
         <v>22.400000000000002</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7" t="s">
-        <v>50</v>
+      <c r="H2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1491,35 +1489,35 @@
         <v>5</v>
       </c>
       <c r="F3" s="1">
-        <v>0.372</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G54" si="1">E3*F3</f>
-        <v>1.8599999999999999</v>
-      </c>
-      <c r="H3" s="11" t="s">
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7" t="s">
-        <v>287</v>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6" t="s">
+        <v>284</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>90</v>
+      <c r="C4" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -1535,29 +1533,29 @@
         <f t="shared" si="1"/>
         <v>0.32099999999999995</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7" t="s">
-        <v>50</v>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>93</v>
+        <v>45</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="D5" s="3">
         <v>44</v>
@@ -1573,29 +1571,29 @@
         <f t="shared" si="1"/>
         <v>3.9820000000000002</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>284</v>
-      </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7" t="s">
-        <v>50</v>
+      <c r="H5" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="D6" s="3">
         <v>10</v>
@@ -1611,29 +1609,29 @@
         <f t="shared" si="1"/>
         <v>1.4000000000000001</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8" t="s">
-        <v>285</v>
+      <c r="H6" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7" t="s">
+        <v>282</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>267</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -1649,27 +1647,27 @@
         <f t="shared" si="1"/>
         <v>1.3900000000000001</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="8" t="s">
-        <v>286</v>
+      <c r="H7" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>270</v>
       </c>
       <c r="D8" s="3">
         <v>2</v>
@@ -1685,29 +1683,29 @@
         <f t="shared" si="1"/>
         <v>0.66</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="J8" s="9"/>
-      <c r="K8" s="8" t="s">
-        <v>285</v>
+      <c r="H8" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="J8" s="8"/>
+      <c r="K8" s="7" t="s">
+        <v>282</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>279</v>
+        <v>266</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>276</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
@@ -1723,27 +1721,27 @@
         <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="8" t="s">
-        <v>286</v>
+      <c r="H9" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
@@ -1759,29 +1757,29 @@
         <f t="shared" si="1"/>
         <v>0.46499999999999997</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>19</v>
+      <c r="H10" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="I10" s="2">
         <v>2441322</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7" t="s">
-        <v>288</v>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6" t="s">
+        <v>285</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
@@ -1797,29 +1795,29 @@
         <f t="shared" si="1"/>
         <v>0.38500000000000001</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="I11" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7" t="s">
-        <v>288</v>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6" t="s">
+        <v>285</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
@@ -1835,27 +1833,27 @@
         <f t="shared" si="1"/>
         <v>1.085</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
@@ -1871,27 +1869,27 @@
         <f t="shared" si="1"/>
         <v>1.085</v>
       </c>
-      <c r="H13" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7" t="s">
-        <v>289</v>
+      <c r="H13" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6" t="s">
+        <v>286</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C14" s="2" t="s">
         <v>121</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="D14" s="3">
         <v>1</v>
@@ -1907,27 +1905,27 @@
         <f t="shared" si="1"/>
         <v>52.75</v>
       </c>
-      <c r="H14" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7" t="s">
-        <v>50</v>
+      <c r="H14" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="17" t="s">
         <v>126</v>
-      </c>
-      <c r="C15" t="s">
-        <v>127</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
@@ -1943,27 +1941,27 @@
         <f t="shared" si="1"/>
         <v>1.24</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="11" t="s">
+      <c r="H15" s="6"/>
+      <c r="I15" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7" t="s">
-        <v>129</v>
-      </c>
       <c r="L15" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="D16" s="3">
         <v>1</v>
@@ -1979,27 +1977,27 @@
         <f t="shared" si="1"/>
         <v>1.1500000000000001</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7" t="s">
-        <v>50</v>
+      <c r="H16" s="6"/>
+      <c r="I16" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>137</v>
+        <v>45</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="D17" s="3">
         <v>2</v>
@@ -2015,29 +2013,29 @@
         <f t="shared" si="1"/>
         <v>3.37</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7" t="s">
-        <v>290</v>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="D18" s="3">
         <v>2</v>
@@ -2053,29 +2051,29 @@
         <f t="shared" si="1"/>
         <v>2.06</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H18" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="I18" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="I18" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7" t="s">
-        <v>50</v>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>146</v>
+        <v>45</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
@@ -2091,29 +2089,29 @@
         <f t="shared" si="1"/>
         <v>1.6500000000000001</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I19" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="I19" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7" t="s">
-        <v>50</v>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>149</v>
+        <v>45</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
@@ -2129,29 +2127,29 @@
         <f t="shared" si="1"/>
         <v>0.96</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="I20" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="I20" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7" t="s">
-        <v>50</v>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>194</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
@@ -2167,29 +2165,29 @@
         <f t="shared" si="1"/>
         <v>0.42500000000000004</v>
       </c>
-      <c r="H21" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7" t="s">
-        <v>291</v>
+      <c r="H21" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6" t="s">
+        <v>288</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>292</v>
+        <v>262</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>289</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
@@ -2205,29 +2203,29 @@
         <f t="shared" si="1"/>
         <v>3.5049999999999999</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="I22" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="7" t="s">
-        <v>295</v>
+      <c r="H22" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="J22" s="8"/>
+      <c r="K22" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
@@ -2243,27 +2241,27 @@
         <f t="shared" si="1"/>
         <v>2.09</v>
       </c>
-      <c r="H23" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7" t="s">
-        <v>296</v>
+      <c r="H23" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6" t="s">
+        <v>293</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>166</v>
+        <v>125</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
@@ -2279,27 +2277,27 @@
         <f t="shared" si="1"/>
         <v>0.99500000000000011</v>
       </c>
-      <c r="H24" s="7"/>
-      <c r="I24" s="11" t="s">
+      <c r="H24" s="6"/>
+      <c r="I24" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>308</v>
+        <v>123</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>305</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
@@ -2315,29 +2313,29 @@
         <f t="shared" si="1"/>
         <v>3.6749999999999998</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="I25" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7" t="s">
-        <v>312</v>
-      </c>
       <c r="L25" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="D26" s="3">
         <v>1</v>
@@ -2353,27 +2351,27 @@
         <f t="shared" si="1"/>
         <v>2.3400000000000003</v>
       </c>
-      <c r="H26" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7" t="s">
-        <v>306</v>
+      <c r="H26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6" t="s">
+        <v>303</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C27" s="2" t="s">
         <v>160</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
@@ -2389,27 +2387,27 @@
         <f t="shared" si="1"/>
         <v>11.45</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="L27" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="D28" s="3">
         <v>6</v>
@@ -2425,29 +2423,29 @@
         <f t="shared" si="1"/>
         <v>7.68</v>
       </c>
-      <c r="H28" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7" t="s">
-        <v>299</v>
+      <c r="H28" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6" t="s">
+        <v>296</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>51</v>
+        <v>16</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="D29" s="3">
         <v>1</v>
@@ -2463,29 +2461,29 @@
         <f t="shared" si="1"/>
         <v>0.505</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I29" s="12" t="s">
+      <c r="H29" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8" t="s">
-        <v>299</v>
+      <c r="I29" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7" t="s">
+        <v>296</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>253</v>
+        <v>204</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>250</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -2501,29 +2499,29 @@
         <f>E30*F30</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H30" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="J30" s="7"/>
-      <c r="K30" s="8" t="s">
-        <v>300</v>
+      <c r="H30" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="J30" s="6"/>
+      <c r="K30" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>249</v>
+        <v>204</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>246</v>
       </c>
       <c r="D31" s="3">
         <v>6</v>
@@ -2539,29 +2537,29 @@
         <f t="shared" si="1"/>
         <v>0.42</v>
       </c>
-      <c r="H31" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="J31" s="7"/>
-      <c r="K31" s="8" t="s">
-        <v>300</v>
+      <c r="H31" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="J31" s="6"/>
+      <c r="K31" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>245</v>
+        <v>204</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>242</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
@@ -2577,29 +2575,29 @@
         <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H32" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="J32" s="7"/>
-      <c r="K32" s="8" t="s">
-        <v>300</v>
+      <c r="H32" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="J32" s="6"/>
+      <c r="K32" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>241</v>
+        <v>204</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>238</v>
       </c>
       <c r="D33" s="3">
         <v>1</v>
@@ -2615,29 +2613,29 @@
         <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H33" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="J33" s="7"/>
-      <c r="K33" s="8" t="s">
-        <v>300</v>
+      <c r="H33" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="J33" s="6"/>
+      <c r="K33" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>237</v>
+        <v>204</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>234</v>
       </c>
       <c r="D34" s="3">
         <v>5</v>
@@ -2653,29 +2651,29 @@
         <f t="shared" si="1"/>
         <v>0.35000000000000003</v>
       </c>
-      <c r="H34" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="J34" s="7"/>
-      <c r="K34" s="8" t="s">
-        <v>300</v>
+      <c r="H34" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="J34" s="6"/>
+      <c r="K34" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>233</v>
+        <v>204</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>230</v>
       </c>
       <c r="D35" s="3">
         <v>1</v>
@@ -2691,29 +2689,29 @@
         <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H35" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="J35" s="7"/>
-      <c r="K35" s="8" t="s">
-        <v>300</v>
+      <c r="H35" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="J35" s="6"/>
+      <c r="K35" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>229</v>
+        <v>204</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>226</v>
       </c>
       <c r="D36" s="3">
         <v>1</v>
@@ -2729,29 +2727,29 @@
         <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H36" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="J36" s="7"/>
-      <c r="K36" s="8" t="s">
-        <v>300</v>
+      <c r="H36" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="J36" s="6"/>
+      <c r="K36" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>224</v>
+        <v>204</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>221</v>
       </c>
       <c r="D37" s="3">
         <v>2</v>
@@ -2767,29 +2765,29 @@
         <f t="shared" si="1"/>
         <v>0.14000000000000001</v>
       </c>
-      <c r="H37" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="J37" s="7"/>
-      <c r="K37" s="8" t="s">
-        <v>300</v>
+      <c r="H37" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="J37" s="6"/>
+      <c r="K37" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>220</v>
+        <v>204</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>217</v>
       </c>
       <c r="D38" s="3">
         <v>1</v>
@@ -2805,29 +2803,29 @@
         <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H38" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="J38" s="7"/>
-      <c r="K38" s="8" t="s">
-        <v>300</v>
+      <c r="H38" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="J38" s="6"/>
+      <c r="K38" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>217</v>
+        <v>204</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>214</v>
       </c>
       <c r="D39" s="3">
         <v>3</v>
@@ -2843,29 +2841,29 @@
         <f t="shared" si="1"/>
         <v>0.21</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="H39" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="I39" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="I39" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J39" s="7"/>
-      <c r="K39" s="8" t="s">
-        <v>300</v>
+      <c r="J39" s="6"/>
+      <c r="K39" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>210</v>
       </c>
       <c r="D40" s="3">
         <v>7</v>
@@ -2881,29 +2879,29 @@
         <f t="shared" si="1"/>
         <v>0.49</v>
       </c>
-      <c r="H40" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="J40" s="7"/>
-      <c r="K40" s="8" t="s">
-        <v>300</v>
+      <c r="H40" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="J40" s="6"/>
+      <c r="K40" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="D41" s="3">
         <v>3</v>
@@ -2919,29 +2917,29 @@
         <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
-      <c r="H41" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J41" s="7"/>
-      <c r="K41" s="8" t="s">
-        <v>300</v>
+      <c r="H41" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="J41" s="6"/>
+      <c r="K41" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>200</v>
       </c>
       <c r="D42" s="3">
         <v>2</v>
@@ -2957,29 +2955,29 @@
         <f t="shared" si="1"/>
         <v>2.79</v>
       </c>
-      <c r="H42" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="I42" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7" t="s">
-        <v>301</v>
+      <c r="H42" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="D43" s="3">
         <v>1</v>
@@ -2989,34 +2987,34 @@
         <v>5</v>
       </c>
       <c r="F43" s="1">
-        <v>0.38</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="G43" s="1">
         <f t="shared" si="1"/>
-        <v>1.9</v>
-      </c>
-      <c r="H43" s="7" t="s">
+        <v>2.335</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I43" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="I43" s="11" t="s">
+      <c r="J43" s="6"/>
+      <c r="K43" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="L43" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D44" s="3">
@@ -3033,27 +3031,27 @@
         <f t="shared" si="1"/>
         <v>60.300000000000004</v>
       </c>
-      <c r="H44" s="11" t="s">
+      <c r="H44" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7" t="s">
-        <v>50</v>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>190</v>
+      <c r="C45" s="6" t="s">
+        <v>187</v>
       </c>
       <c r="D45" s="3">
         <v>5</v>
@@ -3070,27 +3068,27 @@
         <f t="shared" si="1"/>
         <v>32.5</v>
       </c>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="K45" s="7" t="s">
-        <v>50</v>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>155</v>
+        <v>45</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>154</v>
       </c>
       <c r="D46" s="3">
         <v>5</v>
@@ -3106,29 +3104,29 @@
         <f t="shared" si="1"/>
         <v>5.9249999999999998</v>
       </c>
-      <c r="H46" s="11" t="s">
+      <c r="H46" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="I46" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="I46" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7" t="s">
-        <v>302</v>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6" t="s">
+        <v>299</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>156</v>
+        <v>45</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="D47" s="3">
         <v>5</v>
@@ -3144,29 +3142,29 @@
         <f t="shared" si="1"/>
         <v>2.65</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="H47" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="I47" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="I47" s="11" t="s">
+      <c r="J47" s="6"/>
+      <c r="K47" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L47" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>188</v>
+        <v>23</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>185</v>
       </c>
       <c r="D48" s="3">
         <v>1</v>
@@ -3182,27 +3180,27 @@
         <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
-      <c r="H48" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7" t="s">
-        <v>191</v>
+      <c r="H48" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6" t="s">
+        <v>188</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="D49" s="3">
         <v>1</v>
@@ -3218,29 +3216,29 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-      <c r="H49" s="7" t="s">
+      <c r="H49" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="I49" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="J49" s="6"/>
+      <c r="K49" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L49" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="I49" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="J49" s="7"/>
-      <c r="K49" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D50" s="3">
         <v>1</v>
@@ -3256,29 +3254,29 @@
         <f t="shared" si="1"/>
         <v>1.55</v>
       </c>
-      <c r="H50" s="10" t="s">
+      <c r="H50" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I50" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I50" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="J50" s="10"/>
-      <c r="K50" s="17" t="s">
-        <v>303</v>
+      <c r="J50" s="9"/>
+      <c r="K50" s="16" t="s">
+        <v>300</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D51" s="3">
         <v>1</v>
@@ -3294,29 +3292,29 @@
         <f t="shared" si="1"/>
         <v>10.3</v>
       </c>
-      <c r="H51" s="11" t="s">
+      <c r="H51" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I51" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I51" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7" t="s">
-        <v>193</v>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6" t="s">
+        <v>190</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="D52" s="3">
         <v>1</v>
@@ -3332,27 +3330,27 @@
         <f t="shared" si="1"/>
         <v>17.399999999999999</v>
       </c>
-      <c r="H52" s="11" t="s">
-        <v>178</v>
+      <c r="H52" s="10" t="s">
+        <v>175</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="3">
@@ -3369,29 +3367,29 @@
         <f t="shared" si="1"/>
         <v>6.2</v>
       </c>
-      <c r="H53" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I53" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J53" s="7"/>
-      <c r="K53" s="17" t="s">
-        <v>303</v>
+      <c r="H53" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J53" s="6"/>
+      <c r="K53" s="16" t="s">
+        <v>300</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>312</v>
       </c>
       <c r="D54" s="3">
         <v>1</v>
@@ -3401,27 +3399,27 @@
         <v>5</v>
       </c>
       <c r="F54" s="1">
-        <v>0.35599999999999998</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="G54" s="1">
         <f t="shared" si="1"/>
-        <v>1.7799999999999998</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>174</v>
+        <v>2.0100000000000002</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>313</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F56" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="G56" s="16">
+        <v>260</v>
+      </c>
+      <c r="G56" s="15">
         <v>5</v>
       </c>
     </row>
@@ -3431,16 +3429,16 @@
       </c>
       <c r="G57" s="5">
         <f>SUM(G2:G55)</f>
-        <v>291.58299999999991</v>
+        <v>292.02799999999996</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F58" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G58" s="5">
         <f>G57/G56</f>
-        <v>58.31659999999998</v>
+        <v>58.405599999999993</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Switch R19 to 1210, 62R resistor
This allows the speaker to run at 0.35W instead of the previous 0.11W.
</commit_message>
<xml_diff>
--- a/hardware/Parts List.xlsx
+++ b/hardware/Parts List.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="314">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -706,18 +706,6 @@
     <t>9238565</t>
   </si>
   <si>
-    <t>Resistor 220R, 100mW, 75V, +/-1%, SMD 0603</t>
-  </si>
-  <si>
-    <t>RC0603FR-07220RL</t>
-  </si>
-  <si>
-    <t>603-RC0603FR-07220RL</t>
-  </si>
-  <si>
-    <t>9238409</t>
-  </si>
-  <si>
     <t>Resistor 1kR, 100mW, 75V, +/-1%, SMD 0603</t>
   </si>
   <si>
@@ -959,6 +947,18 @@
   </si>
   <si>
     <t xml:space="preserve">449-LFXTAL027945REEL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC1210FR-0762RL </t>
+  </si>
+  <si>
+    <t>Resistor 62R, 500mW, 75V, +/-1%, SMD 1210</t>
+  </si>
+  <si>
+    <t>RC1210FR-0762RL</t>
+  </si>
+  <si>
+    <t>Resistor_SMD:R_1210_3225Metric_Pad1.42x2.65mm_HandSolder</t>
   </si>
 </sst>
 </file>
@@ -1374,9 +1374,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,13 +1406,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -1468,7 +1468,7 @@
         <v>49</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>113</v>
@@ -1572,28 +1572,28 @@
         <v>3.9820000000000002</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
         <v>49</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D6" s="3">
         <v>10</v>
@@ -1610,17 +1610,17 @@
         <v>1.4000000000000001</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1628,10 +1628,10 @@
         <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -1648,15 +1648,15 @@
         <v>1.3900000000000001</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="7" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1664,10 +1664,10 @@
         <v>54</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D8" s="3">
         <v>2</v>
@@ -1684,17 +1684,17 @@
         <v>0.66</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="7" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1702,10 +1702,10 @@
         <v>55</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
@@ -1722,15 +1722,15 @@
         <v>1.2</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="7" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>112</v>
@@ -1803,7 +1803,7 @@
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>111</v>
@@ -1839,7 +1839,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>110</v>
@@ -1875,7 +1875,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>114</v>
@@ -2021,7 +2021,7 @@
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>118</v>
@@ -2173,7 +2173,7 @@
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>197</v>
@@ -2184,10 +2184,10 @@
         <v>73</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
@@ -2204,14 +2204,14 @@
         <v>3.5049999999999999</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>168</v>
@@ -2247,7 +2247,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>170</v>
@@ -2283,7 +2283,7 @@
       </c>
       <c r="J24" s="6"/>
       <c r="K24" s="6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>167</v>
@@ -2297,7 +2297,7 @@
         <v>123</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
@@ -2314,17 +2314,17 @@
         <v>3.6749999999999998</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="6" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2357,7 +2357,7 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>115</v>
@@ -2393,7 +2393,7 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>162</v>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="6" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>116</v>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="J29" s="7"/>
       <c r="K29" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>117</v>
@@ -2483,7 +2483,7 @@
         <v>204</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -2500,17 +2500,17 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="J30" s="6"/>
       <c r="K30" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2521,7 +2521,7 @@
         <v>204</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D31" s="3">
         <v>6</v>
@@ -2538,17 +2538,17 @@
         <v>0.42</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2559,7 +2559,7 @@
         <v>204</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
@@ -2576,17 +2576,17 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2597,7 +2597,7 @@
         <v>204</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D33" s="3">
         <v>1</v>
@@ -2614,28 +2614,28 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>204</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D34" s="3">
         <v>5</v>
@@ -2652,17 +2652,17 @@
         <v>0.35000000000000003</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2673,7 +2673,7 @@
         <v>204</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>230</v>
+        <v>312</v>
       </c>
       <c r="D35" s="3">
         <v>1</v>
@@ -2683,24 +2683,22 @@
         <v>5</v>
       </c>
       <c r="F35" s="1">
-        <v>1.4E-2</v>
+        <v>0.122</v>
       </c>
       <c r="G35" s="1">
         <f t="shared" si="1"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="H35" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>232</v>
-      </c>
+        <v>0.61</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="I35" s="6"/>
       <c r="J35" s="6"/>
       <c r="K35" s="7" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>229</v>
+        <v>311</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2735,7 +2733,7 @@
       </c>
       <c r="J36" s="6"/>
       <c r="K36" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>225</v>
@@ -2773,7 +2771,7 @@
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>220</v>
@@ -2811,7 +2809,7 @@
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>216</v>
@@ -2849,7 +2847,7 @@
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="L39" s="2" t="s">
         <v>213</v>
@@ -2887,7 +2885,7 @@
       </c>
       <c r="J40" s="6"/>
       <c r="K40" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="L40" s="2" t="s">
         <v>209</v>
@@ -2925,7 +2923,7 @@
       </c>
       <c r="J41" s="6"/>
       <c r="K41" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="L41" s="2" t="s">
         <v>208</v>
@@ -2963,7 +2961,7 @@
       </c>
       <c r="J42" s="6"/>
       <c r="K42" s="6" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>203</v>
@@ -3040,7 +3038,7 @@
         <v>49</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -3071,13 +3069,13 @@
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
       <c r="J45" s="13" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="K45" s="6" t="s">
         <v>49</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -3112,7 +3110,7 @@
       </c>
       <c r="J46" s="6"/>
       <c r="K46" s="6" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>119</v>
@@ -3262,7 +3260,7 @@
       </c>
       <c r="J50" s="9"/>
       <c r="K50" s="16" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>189</v>
@@ -3337,7 +3335,7 @@
         <v>176</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>177</v>
@@ -3368,14 +3366,14 @@
         <v>6.2</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>15</v>
       </c>
       <c r="J53" s="6"/>
       <c r="K53" s="16" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="L53" s="2" t="s">
         <v>192</v>
@@ -3389,7 +3387,7 @@
         <v>171</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D54" s="3">
         <v>1</v>
@@ -3406,10 +3404,10 @@
         <v>2.0100000000000002</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>172</v>
@@ -3417,7 +3415,7 @@
     </row>
     <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F56" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="G56" s="15">
         <v>5</v>
@@ -3429,16 +3427,16 @@
       </c>
       <c r="G57" s="5">
         <f>SUM(G2:G55)</f>
-        <v>292.02799999999996</v>
+        <v>292.56799999999998</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F58" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G58" s="5">
         <f>G57/G56</f>
-        <v>58.405599999999993</v>
+        <v>58.513599999999997</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>